<commit_message>
Changes after profile delete on VM
</commit_message>
<xml_diff>
--- a/TestData/TMTT0011411_Verify_user_with_Title_TAG_Outsourced_Contractor.xlsx
+++ b/TestData/TMTT0011411_Verify_user_with_Title_TAG_Outsourced_Contractor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5CCE62-72C9-4CEF-9398-6AD19F6B0A7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28679F53-C288-4AFC-A6F1-2077824B3A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18420" windowHeight="5760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="8" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>TAG Analyst</t>
   </si>
   <si>
-    <t>E-Bartush-FVA-110095</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Fieldwork</t>
   </si>
   <si>
-    <t>Engagement Project Wildcat-FVA-108747</t>
-  </si>
-  <si>
     <t>Future Time Period Activity List</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>Summary_Log</t>
+  </si>
+  <si>
+    <t>Bartush-Cotton Creek Capital Management LLC-FVA-110095</t>
+  </si>
+  <si>
+    <t>Project Wildcat-Ares Management LLC-FVA-108747</t>
   </si>
 </sst>
 </file>
@@ -786,10 +786,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -811,22 +814,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="50.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -838,29 +841,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -873,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -884,12 +888,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -903,7 +907,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,19 +917,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -939,26 +943,26 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>